<commit_message>
update abc_acl mackerel and productivity
</commit_message>
<xml_diff>
--- a/data-raw/ABC_ACL_catch - Brandon Muffley - NOAA Affiliate.xlsx
+++ b/data-raw/ABC_ACL_catch - Brandon Muffley - NOAA Affiliate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22950" windowHeight="11205"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="MAFMC ABC_ACL_catch" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -641,77 +641,80 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1031,7 +1034,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S2" sqref="S2"/>
+      <selection pane="topRight" activeCell="R11" sqref="R11:R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,42 +1056,42 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="58">
+      <c r="B1" s="78">
         <v>2012</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="58">
+      <c r="C1" s="79"/>
+      <c r="D1" s="78">
         <v>2013</v>
       </c>
-      <c r="E1" s="59"/>
-      <c r="F1" s="58">
+      <c r="E1" s="80"/>
+      <c r="F1" s="78">
         <v>2014</v>
       </c>
-      <c r="G1" s="59"/>
-      <c r="H1" s="58">
+      <c r="G1" s="80"/>
+      <c r="H1" s="78">
         <v>2015</v>
       </c>
-      <c r="I1" s="59"/>
-      <c r="J1" s="58">
+      <c r="I1" s="80"/>
+      <c r="J1" s="78">
         <v>2016</v>
       </c>
-      <c r="K1" s="59"/>
-      <c r="L1" s="58">
+      <c r="K1" s="80"/>
+      <c r="L1" s="78">
         <v>2017</v>
       </c>
-      <c r="M1" s="59"/>
-      <c r="N1" s="58">
+      <c r="M1" s="80"/>
+      <c r="N1" s="78">
         <v>2018</v>
       </c>
-      <c r="O1" s="60"/>
-      <c r="P1" s="58">
+      <c r="O1" s="81"/>
+      <c r="P1" s="78">
         <v>2019</v>
       </c>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="58">
+      <c r="Q1" s="81"/>
+      <c r="R1" s="78">
         <v>2020</v>
       </c>
-      <c r="S1" s="61"/>
+      <c r="S1" s="79"/>
       <c r="T1" s="2"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1681,55 +1684,55 @@
       <c r="A11" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="62">
+      <c r="B11" s="82">
         <v>80000</v>
       </c>
       <c r="C11" s="24">
         <v>2670</v>
       </c>
-      <c r="D11" s="62">
+      <c r="D11" s="82">
         <v>80000</v>
       </c>
       <c r="E11" s="24">
         <v>2406</v>
       </c>
-      <c r="F11" s="62">
+      <c r="F11" s="82">
         <v>80000</v>
       </c>
       <c r="G11" s="24">
         <v>2296</v>
       </c>
-      <c r="H11" s="62">
+      <c r="H11" s="82">
         <v>40165</v>
       </c>
       <c r="I11" s="24">
         <v>4274</v>
       </c>
-      <c r="J11" s="62">
+      <c r="J11" s="82">
         <v>19898</v>
       </c>
       <c r="K11" s="16">
         <v>4569</v>
       </c>
-      <c r="L11" s="62">
+      <c r="L11" s="82">
         <v>19898</v>
       </c>
       <c r="M11" s="11">
         <v>4161</v>
       </c>
-      <c r="N11" s="62">
+      <c r="N11" s="82">
         <v>19898</v>
       </c>
       <c r="O11" s="11">
         <v>2394</v>
       </c>
-      <c r="P11" s="62">
+      <c r="P11" s="82">
         <v>29184</v>
       </c>
       <c r="Q11" s="11">
         <v>2117</v>
       </c>
-      <c r="R11" s="62">
+      <c r="R11" s="82">
         <v>29184</v>
       </c>
       <c r="S11" s="31">
@@ -1743,42 +1746,60 @@
       <c r="A12" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="63"/>
+      <c r="B12" s="82">
+        <v>80000</v>
+      </c>
       <c r="C12" s="16">
         <f>5333+33</f>
         <v>5366</v>
       </c>
-      <c r="D12" s="63"/>
+      <c r="D12" s="82">
+        <v>80000</v>
+      </c>
       <c r="E12" s="16">
         <f>4372+20</f>
         <v>4392</v>
       </c>
-      <c r="F12" s="63"/>
+      <c r="F12" s="82">
+        <v>80000</v>
+      </c>
       <c r="G12" s="16">
         <f>5905+51</f>
         <v>5956</v>
       </c>
-      <c r="H12" s="63"/>
+      <c r="H12" s="82">
+        <v>40165</v>
+      </c>
       <c r="I12" s="16">
         <v>5629</v>
       </c>
-      <c r="J12" s="63"/>
+      <c r="J12" s="82">
+        <v>19898</v>
+      </c>
       <c r="K12" s="18">
         <v>5705</v>
       </c>
-      <c r="L12" s="63"/>
+      <c r="L12" s="82">
+        <v>19898</v>
+      </c>
       <c r="M12" s="12">
         <v>7058</v>
       </c>
-      <c r="N12" s="63"/>
+      <c r="N12" s="82">
+        <v>19898</v>
+      </c>
       <c r="O12" s="12">
         <v>8894</v>
       </c>
-      <c r="P12" s="63"/>
+      <c r="P12" s="82">
+        <v>29184</v>
+      </c>
       <c r="Q12" s="12">
         <v>5579</v>
       </c>
-      <c r="R12" s="63"/>
+      <c r="R12" s="82">
+        <v>29184</v>
+      </c>
       <c r="S12" s="32">
         <v>8219</v>
       </c>
@@ -2124,190 +2145,190 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="72" t="s">
+      <c r="A19" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="67">
+      <c r="B19" s="72">
         <v>32.04</v>
       </c>
-      <c r="C19" s="67">
+      <c r="C19" s="72">
         <v>19.260000000000002</v>
       </c>
-      <c r="D19" s="67">
+      <c r="D19" s="72">
         <v>27.47</v>
       </c>
-      <c r="E19" s="67">
+      <c r="E19" s="72">
         <v>24.06</v>
       </c>
-      <c r="F19" s="67">
+      <c r="F19" s="72">
         <v>24.43</v>
       </c>
-      <c r="G19" s="67">
+      <c r="G19" s="72">
         <v>17.96</v>
       </c>
-      <c r="H19" s="67">
+      <c r="H19" s="72">
         <v>21.54</v>
       </c>
-      <c r="I19" s="67">
+      <c r="I19" s="72">
         <v>18.649999999999999</v>
       </c>
-      <c r="J19" s="67">
+      <c r="J19" s="72">
         <v>19.45</v>
       </c>
-      <c r="K19" s="67">
+      <c r="K19" s="72">
         <v>16.09</v>
       </c>
-      <c r="L19" s="70">
+      <c r="L19" s="76">
         <v>20.64</v>
       </c>
-      <c r="M19" s="70">
+      <c r="M19" s="76">
         <v>15.65</v>
       </c>
-      <c r="N19" s="70">
+      <c r="N19" s="76">
         <v>21.81</v>
       </c>
-      <c r="O19" s="70">
+      <c r="O19" s="76">
         <v>6.96</v>
       </c>
-      <c r="P19" s="70">
+      <c r="P19" s="76">
         <v>21.81</v>
       </c>
-      <c r="Q19" s="70">
+      <c r="Q19" s="76">
         <v>23.5</v>
       </c>
-      <c r="R19" s="70">
+      <c r="R19" s="76">
         <v>16.28</v>
       </c>
-      <c r="S19" s="80">
+      <c r="S19" s="65">
         <v>15.74</v>
       </c>
-      <c r="T19" s="74" t="s">
+      <c r="T19" s="58" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="73"/>
-      <c r="B20" s="68"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="68"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="68"/>
-      <c r="K20" s="68"/>
-      <c r="L20" s="71"/>
-      <c r="M20" s="71"/>
-      <c r="N20" s="71"/>
-      <c r="O20" s="71"/>
-      <c r="P20" s="71"/>
-      <c r="Q20" s="71"/>
-      <c r="R20" s="71"/>
-      <c r="S20" s="81"/>
-      <c r="T20" s="75"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="73"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
+      <c r="H20" s="73"/>
+      <c r="I20" s="73"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="73"/>
+      <c r="L20" s="63"/>
+      <c r="M20" s="63"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="63"/>
+      <c r="P20" s="63"/>
+      <c r="Q20" s="63"/>
+      <c r="R20" s="63"/>
+      <c r="S20" s="66"/>
+      <c r="T20" s="59"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="67" t="s">
+      <c r="A21" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="62">
+      <c r="B21" s="69">
         <v>20352</v>
       </c>
       <c r="C21" s="24">
         <v>10660</v>
       </c>
-      <c r="D21" s="62">
+      <c r="D21" s="69">
         <v>24709</v>
       </c>
       <c r="E21" s="24">
         <v>7312</v>
       </c>
-      <c r="F21" s="62">
+      <c r="F21" s="69">
         <v>27596</v>
       </c>
       <c r="G21" s="24">
         <v>10651</v>
       </c>
-      <c r="H21" s="62">
+      <c r="H21" s="69">
         <v>28310</v>
       </c>
       <c r="I21" s="24">
         <v>8663</v>
       </c>
-      <c r="J21" s="62">
+      <c r="J21" s="69">
         <v>23617</v>
       </c>
       <c r="K21" s="24">
         <v>12097</v>
       </c>
-      <c r="L21" s="78">
+      <c r="L21" s="62">
         <v>23045</v>
       </c>
       <c r="M21" s="24">
         <v>8735</v>
       </c>
-      <c r="N21" s="79">
+      <c r="N21" s="64">
         <v>22635</v>
       </c>
       <c r="O21" s="24">
         <v>6878</v>
       </c>
-      <c r="P21" s="79">
+      <c r="P21" s="64">
         <v>12914</v>
       </c>
       <c r="Q21" s="24">
         <v>8642.7729041739622</v>
       </c>
-      <c r="R21" s="79">
+      <c r="R21" s="64">
         <v>14126</v>
       </c>
       <c r="S21" s="24">
         <v>5790.3715833114102</v>
       </c>
-      <c r="T21" s="76" t="s">
+      <c r="T21" s="60" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="71"/>
-      <c r="B22" s="63"/>
+      <c r="A22" s="63"/>
+      <c r="B22" s="71"/>
       <c r="C22" s="16">
         <v>45</v>
       </c>
-      <c r="D22" s="69"/>
+      <c r="D22" s="70"/>
       <c r="E22" s="16">
         <v>67</v>
       </c>
-      <c r="F22" s="69"/>
+      <c r="F22" s="70"/>
       <c r="G22" s="16">
         <v>108</v>
       </c>
-      <c r="H22" s="69"/>
+      <c r="H22" s="70"/>
       <c r="I22" s="16">
         <v>44</v>
       </c>
-      <c r="J22" s="69"/>
+      <c r="J22" s="70"/>
       <c r="K22" s="16">
         <v>141</v>
       </c>
-      <c r="L22" s="71"/>
+      <c r="L22" s="63"/>
       <c r="M22" s="16">
         <v>130</v>
       </c>
-      <c r="N22" s="71"/>
+      <c r="N22" s="63"/>
       <c r="O22" s="16">
         <v>35</v>
       </c>
-      <c r="P22" s="71"/>
+      <c r="P22" s="63"/>
       <c r="Q22" s="16">
         <v>53</v>
       </c>
-      <c r="R22" s="71"/>
+      <c r="R22" s="63"/>
       <c r="S22" s="16">
         <v>120</v>
       </c>
-      <c r="T22" s="77"/>
+      <c r="T22" s="61"/>
     </row>
     <row r="23" spans="1:20" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
@@ -2417,53 +2438,32 @@
       <c r="B29" s="43"/>
     </row>
     <row r="35" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F35" s="64"/>
-      <c r="G35" s="64"/>
-      <c r="H35" s="64"/>
-      <c r="I35" s="64"/>
-      <c r="J35" s="66"/>
-      <c r="K35" s="64"/>
+      <c r="F35" s="74"/>
+      <c r="G35" s="74"/>
+      <c r="H35" s="74"/>
+      <c r="I35" s="74"/>
+      <c r="J35" s="77"/>
+      <c r="K35" s="74"/>
     </row>
     <row r="36" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F36" s="65"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="65"/>
-      <c r="I36" s="65"/>
-      <c r="J36" s="65"/>
-      <c r="K36" s="65"/>
+      <c r="F36" s="75"/>
+      <c r="G36" s="75"/>
+      <c r="H36" s="75"/>
+      <c r="I36" s="75"/>
+      <c r="J36" s="75"/>
+      <c r="K36" s="75"/>
     </row>
   </sheetData>
-  <mergeCells count="55">
-    <mergeCell ref="T19:T20"/>
-    <mergeCell ref="T21:T22"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="P21:P22"/>
-    <mergeCell ref="R21:R22"/>
-    <mergeCell ref="S19:S20"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="R19:R20"/>
-    <mergeCell ref="J11:J12"/>
+  <mergeCells count="46">
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="F35:F36"/>
     <mergeCell ref="G35:G36"/>
     <mergeCell ref="H35:H36"/>
@@ -2476,19 +2476,31 @@
     <mergeCell ref="J19:J20"/>
     <mergeCell ref="H21:H22"/>
     <mergeCell ref="J21:J22"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="R19:R20"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="T19:T20"/>
+    <mergeCell ref="T21:T22"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="R21:R22"/>
+    <mergeCell ref="S19:S20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2739,18 +2751,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2773,6 +2785,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D9A4291-A5FA-41C6-97E5-6A144A24C689}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1D4F6EF-82E5-49BC-AA19-CDCD9BB9760B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2787,12 +2807,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D9A4291-A5FA-41C6-97E5-6A144A24C689}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>